<commit_message>
COmpletely reworked the Spiral function from scratch, and added spiral plots to the final diagram.
</commit_message>
<xml_diff>
--- a/JupyterNotebooks/AveragedIntensites/alpha1F-HW10.xlsx
+++ b/JupyterNotebooks/AveragedIntensites/alpha1F-HW10.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="alpha1F-HW10.xpc" sheetId="1" r:id="rId1"/>
+    <sheet name="alpha1F" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -949,16 +949,16 @@
         <v>11</v>
       </c>
       <c r="C13">
-        <v>0.9894216124101329</v>
+        <v>0.9894216124101333</v>
       </c>
       <c r="D13">
-        <v>0.9939417127373232</v>
+        <v>0.9939417127373235</v>
       </c>
       <c r="E13">
-        <v>0.9907191400909074</v>
+        <v>0.9907191400909077</v>
       </c>
       <c r="F13">
-        <v>0.9894216124101329</v>
+        <v>0.9894216124101333</v>
       </c>
       <c r="G13">
         <v>1.001245482278839</v>
@@ -970,16 +970,16 @@
         <v>0.9923555296373245</v>
       </c>
       <c r="J13">
-        <v>0.9939417127373232</v>
+        <v>0.9939417127373235</v>
       </c>
       <c r="K13">
-        <v>0.9923304264141153</v>
+        <v>0.9923304264141155</v>
       </c>
       <c r="L13">
-        <v>0.9908760194121241</v>
+        <v>0.9908760194121244</v>
       </c>
       <c r="M13">
-        <v>0.9924318806143937</v>
+        <v>0.992431880614394</v>
       </c>
     </row>
     <row r="14" spans="1:13">

</xml_diff>